<commit_message>
Add some format and enable typing file name
</commit_message>
<xml_diff>
--- a/test02.xlsx
+++ b/test02.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -313,13 +313,20 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -347,15 +354,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -429,6 +441,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -463,6 +476,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -638,883 +652,892 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C79"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="89.140625" customWidth="1"/>
+    <col min="3" max="3" width="47.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
         <v>17</v>
       </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
         <v>18</v>
       </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
         <v>19</v>
       </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
         <v>20</v>
       </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
         <v>21</v>
       </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
         <v>22</v>
       </c>
-      <c r="C17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
         <v>23</v>
       </c>
-      <c r="C18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
         <v>24</v>
       </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
         <v>25</v>
       </c>
-      <c r="C20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
         <v>26</v>
       </c>
-      <c r="C21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
         <v>27</v>
       </c>
-      <c r="C22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
         <v>28</v>
       </c>
-      <c r="C23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" t="s">
         <v>30</v>
       </c>
-      <c r="C24" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="C26" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" t="s">
         <v>34</v>
       </c>
-      <c r="C27" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
         <v>35</v>
       </c>
-      <c r="C28" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
         <v>36</v>
       </c>
-      <c r="C29" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
         <v>37</v>
       </c>
-      <c r="C30" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
         <v>38</v>
       </c>
-      <c r="C31" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" t="s">
         <v>39</v>
       </c>
-      <c r="C32" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" t="s">
         <v>40</v>
       </c>
-      <c r="C33" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>29</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" t="s">
         <v>41</v>
       </c>
-      <c r="C34" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" t="s">
         <v>42</v>
       </c>
-      <c r="C35" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>29</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" t="s">
         <v>43</v>
       </c>
-      <c r="C36" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>29</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" t="s">
         <v>44</v>
       </c>
-      <c r="C37" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" t="s">
         <v>45</v>
       </c>
-      <c r="C38" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" t="s">
         <v>46</v>
       </c>
-      <c r="C39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" t="s">
-        <v>29</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" t="s">
         <v>47</v>
       </c>
-      <c r="C40" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" t="s">
-        <v>29</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" t="s">
         <v>48</v>
       </c>
-      <c r="C41" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
-        <v>29</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43" t="s">
         <v>49</v>
       </c>
-      <c r="C42" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
-        <v>29</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>29</v>
+      </c>
+      <c r="B44" t="s">
         <v>50</v>
       </c>
-      <c r="C43" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
-        <v>29</v>
-      </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>29</v>
+      </c>
+      <c r="B45" t="s">
         <v>51</v>
       </c>
-      <c r="C44" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
-        <v>29</v>
-      </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>29</v>
+      </c>
+      <c r="B46" t="s">
         <v>52</v>
       </c>
-      <c r="C45" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" t="s">
-        <v>29</v>
-      </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>29</v>
+      </c>
+      <c r="B47" t="s">
         <v>53</v>
       </c>
-      <c r="C46" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" t="s">
-        <v>29</v>
-      </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>29</v>
+      </c>
+      <c r="B48" t="s">
         <v>54</v>
       </c>
-      <c r="C47" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" t="s">
-        <v>29</v>
-      </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>29</v>
+      </c>
+      <c r="B49" t="s">
         <v>55</v>
       </c>
-      <c r="C48" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" t="s">
-        <v>29</v>
-      </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>29</v>
+      </c>
+      <c r="B50" t="s">
         <v>56</v>
       </c>
-      <c r="C49" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" t="s">
-        <v>29</v>
-      </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>29</v>
+      </c>
+      <c r="B51" t="s">
         <v>57</v>
       </c>
-      <c r="C50" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" t="s">
-        <v>29</v>
-      </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>29</v>
+      </c>
+      <c r="B52" t="s">
         <v>58</v>
       </c>
-      <c r="C51" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" t="s">
-        <v>29</v>
-      </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>29</v>
+      </c>
+      <c r="B53" t="s">
         <v>59</v>
       </c>
-      <c r="C52" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" t="s">
-        <v>29</v>
-      </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>29</v>
+      </c>
+      <c r="B54" t="s">
         <v>60</v>
       </c>
-      <c r="C53" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" t="s">
-        <v>29</v>
-      </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>29</v>
+      </c>
+      <c r="B55" t="s">
         <v>61</v>
       </c>
-      <c r="C54" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" t="s">
-        <v>29</v>
-      </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>29</v>
+      </c>
+      <c r="B56" t="s">
         <v>62</v>
       </c>
-      <c r="C55" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" t="s">
-        <v>29</v>
-      </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>29</v>
+      </c>
+      <c r="B57" t="s">
         <v>63</v>
       </c>
-      <c r="C56" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" t="s">
-        <v>29</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>29</v>
+      </c>
+      <c r="B58" t="s">
         <v>64</v>
       </c>
-      <c r="C57" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" t="s">
-        <v>29</v>
-      </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>29</v>
+      </c>
+      <c r="B59" t="s">
         <v>65</v>
       </c>
-      <c r="C58" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" t="s">
-        <v>29</v>
-      </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>29</v>
+      </c>
+      <c r="B60" t="s">
         <v>66</v>
       </c>
-      <c r="C59" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" t="s">
-        <v>67</v>
-      </c>
-      <c r="B60" t="s">
-        <v>68</v>
-      </c>
       <c r="C60" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>67</v>
       </c>
       <c r="B61" t="s">
+        <v>68</v>
+      </c>
+      <c r="C61" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>67</v>
+      </c>
+      <c r="B62" t="s">
         <v>70</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
-      <c r="A62" t="s">
-        <v>72</v>
-      </c>
-      <c r="B62" t="s">
-        <v>73</v>
-      </c>
-      <c r="C62" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>72</v>
       </c>
       <c r="B63" t="s">
+        <v>73</v>
+      </c>
+      <c r="C63" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>72</v>
+      </c>
+      <c r="B64" t="s">
         <v>75</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C64" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
-      <c r="A64" t="s">
-        <v>77</v>
-      </c>
-      <c r="B64" t="s">
-        <v>78</v>
-      </c>
-      <c r="C64" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>77</v>
       </c>
       <c r="B65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C65" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>77</v>
       </c>
       <c r="B66" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C66" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>77</v>
       </c>
       <c r="B67" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C67" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B68" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C68" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>83</v>
       </c>
       <c r="B69" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C69" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B70" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C70" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>87</v>
       </c>
       <c r="B71" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C71" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>87</v>
       </c>
       <c r="B72" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C72" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>87</v>
       </c>
       <c r="B73" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C73" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>87</v>
       </c>
       <c r="B74" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C74" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>87</v>
       </c>
       <c r="B75" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C75" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>87</v>
       </c>
       <c r="B76" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C76" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>87</v>
       </c>
       <c r="B77" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C77" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>87</v>
       </c>
       <c r="B78" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C78" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>87</v>
       </c>
       <c r="B79" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C79" t="s">
         <v>74</v>
       </c>
     </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>87</v>
+      </c>
+      <c r="B80" t="s">
+        <v>97</v>
+      </c>
+      <c r="C80" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>